<commit_message>
ff kijke of het kan
</commit_message>
<xml_diff>
--- a/Grafieken/build.xlsx
+++ b/Grafieken/build.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\OMVISWEG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerben\Documents\OMVISWEG\Grafieken\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Gesorteerd</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Hash</t>
+  </si>
+  <si>
+    <t>Unsorted</t>
+  </si>
+  <si>
+    <t>Sorted</t>
+  </si>
+  <si>
+    <t>Reverse sorted</t>
   </si>
 </sst>
 </file>
@@ -99,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,7 +126,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -363,11 +372,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="170199904"/>
-        <c:axId val="170200464"/>
+        <c:axId val="193050960"/>
+        <c:axId val="193051352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170199904"/>
+        <c:axId val="193050960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +419,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170200464"/>
+        <c:crossAx val="193051352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -418,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170200464"/>
+        <c:axId val="193051352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="700"/>
@@ -471,7 +480,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170199904"/>
+        <c:crossAx val="193050960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -554,7 +563,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -821,11 +830,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="170204384"/>
-        <c:axId val="170204944"/>
+        <c:axId val="193047824"/>
+        <c:axId val="193481088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170204384"/>
+        <c:axId val="193047824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +877,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170204944"/>
+        <c:crossAx val="193481088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -876,7 +885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170204944"/>
+        <c:axId val="193481088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1100"/>
@@ -929,7 +938,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170204384"/>
+        <c:crossAx val="193047824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1013,7 +1022,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1286,11 +1295,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="170208864"/>
-        <c:axId val="170209424"/>
+        <c:axId val="193046648"/>
+        <c:axId val="193481872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170208864"/>
+        <c:axId val="193046648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1342,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170209424"/>
+        <c:crossAx val="193481872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1341,7 +1350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170209424"/>
+        <c:axId val="193481872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1401,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170208864"/>
+        <c:crossAx val="193046648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1476,7 +1485,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1742,11 +1751,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="172140208"/>
-        <c:axId val="172140768"/>
+        <c:axId val="193482656"/>
+        <c:axId val="193483048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172140208"/>
+        <c:axId val="193482656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1798,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172140768"/>
+        <c:crossAx val="193483048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1797,7 +1806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172140768"/>
+        <c:axId val="193483048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1848,7 +1857,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172140208"/>
+        <c:crossAx val="193482656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1931,7 +1940,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2008,7 +2017,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ongesorteerd</c:v>
+                  <c:v>Unsorted</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2097,7 +2106,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gesorteerd</c:v>
+                  <c:v>Sorted</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2186,7 +2195,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Omgekeerd gesorteerd</c:v>
+                  <c:v>Reverse sorted</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2276,11 +2285,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="172144688"/>
-        <c:axId val="172145248"/>
+        <c:axId val="193483832"/>
+        <c:axId val="193484224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172144688"/>
+        <c:axId val="193483832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2320,7 +2329,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172145248"/>
+        <c:crossAx val="193484224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2328,7 +2337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172145248"/>
+        <c:axId val="193484224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2376,7 +2385,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172144688"/>
+        <c:crossAx val="193483832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2449,7 +2458,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -5291,9 +5300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5331,7 +5340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5403,7 +5412,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5556,7 +5565,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5819,13 +5828,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>